<commit_message>
observaciones lab 7 - maquina 2
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2022-20/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majoa\Downloads\LabCollision-L07-INTER-G02\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="726" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F54888-DFB5-49D6-8E23-12D138256747}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74865F3-A749-401A-AE0A-3A05659B2C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="887" windowWidth="2273" windowHeight="1493" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="1450" yWindow="340" windowWidth="14400" windowHeight="7360" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -59,16 +59,16 @@
     <t>Consumo de Datos [kB]</t>
   </si>
   <si>
-    <t>Carga de Catálogo PROBING (-large)</t>
-  </si>
-  <si>
-    <t>Carga de Catálogo CHAINING (-large)</t>
-  </si>
-  <si>
     <t>Tiempo de Ejecución Real @LP [ms]</t>
   </si>
   <si>
     <t>Tiempo de Ejecución Real @SC [ms]</t>
+  </si>
+  <si>
+    <t>Carga de Catálogo PROBING (-50pct)</t>
+  </si>
+  <si>
+    <t>Carga de Catálogo CHAINING (-50pct)</t>
   </si>
 </sst>
 </file>
@@ -115,7 +115,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,18 +124,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -163,40 +157,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,92 +196,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <b val="0"/>
@@ -384,32 +315,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -459,7 +364,937 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de ejecución LP vs SC</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab7'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo de Ejecución Real @SC [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Datos Lab7'!$C$11:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>65300.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54212.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54328.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54949.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E43B-45C8-8C56-9335629AE6B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab7'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo de Ejecución Real @LP [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Datos Lab7'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>179709.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58644.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93826.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84233.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E43B-45C8-8C56-9335629AE6B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1974779232"/>
+        <c:axId val="1986395168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1974779232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1986395168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1986395168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de ejecución  [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1974779232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab7'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Consumo de Datos [kB]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3531.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3531.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3531.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3531.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6F31-4CC4-AE2C-36242BB27D3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab7'!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Consumo de Datos [kB]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3502.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3504.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3506.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3506.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6F31-4CC4-AE2C-36242BB27D3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1974779232"/>
+        <c:axId val="1986395168"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Datos Lab7'!$C$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Tiempo de Ejecución Real @SC [ms]</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Datos Lab7'!$C$11:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>65300.68</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>54212.800000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>54328.05</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>54949.62</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-6F31-4CC4-AE2C-36242BB27D3D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Datos Lab7'!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Tiempo de Ejecución Real @LP [ms]</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Datos Lab7'!$C$3:$C$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>179709.09</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>58644.27</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>93826.36</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>84233.8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-6F31-4CC4-AE2C-36242BB27D3D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1974779232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1986395168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1986395168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1974779232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.705554922064342E-2"/>
+          <c:y val="0.81386746364733609"/>
+          <c:w val="0.87817024679910638"/>
+          <c:h val="8.8351403718514257E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -499,7 +1334,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Ejecución</a:t>
+              <a:t>Ejecución Probing</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -628,19 +1463,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>3531.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -649,19 +1484,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>179709.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>58644.27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>93826.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>84233.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -759,16 +1594,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>3502.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>3504.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3506.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>3506.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,16 +1615,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$11:$C$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>65300.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>54212.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54328.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>54949.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,7 +1726,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1010,7 +1851,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1122,10 +1963,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1343,19 +2184,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>3531.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>3531.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,16 +2342,19 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>3502.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>3504.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3506.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>3506.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1712,7 +2556,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1818,6 +2662,83 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -1854,7 +2775,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -1892,7 +2813,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1919,8 +2840,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2000,6 +2921,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2010,6 +2936,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2021,7 +2952,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2041,6 +2972,1028 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2407,7 +4360,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2890,7 +4843,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CAFD5B44-21B9-42C7-B503-C146EF1BA3EE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="61" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2901,7 +4854,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{680E7371-595A-4F03-ABE3-E0257A96E5F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="61" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2910,9 +4863,88 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>355601</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5B09496-6BA6-A61A-7A51-2B3EDB9AC6C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>463549</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D279F0-150C-4ACA-883A-D9D7AE7F31EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8660984" cy="6287541"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2941,11 +4973,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8660984" cy="6287541"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2975,31 +5007,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
-    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3298,24 +5330,24 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3323,136 +5355,193 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="10">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <v>0.1</v>
       </c>
-      <c r="B3" s="5">
-        <v>100</v>
+      <c r="B3" s="10">
+        <v>3531.66</v>
       </c>
-      <c r="C3" s="8">
-        <v>75</v>
+      <c r="C3" s="11">
+        <v>179709.09</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="11">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
         <v>0.5</v>
       </c>
-      <c r="B4" s="6">
-        <f>B3+40</f>
-        <v>140</v>
+      <c r="B4" s="1">
+        <v>3531.65</v>
       </c>
-      <c r="C4" s="8">
-        <f>C3+10</f>
-        <v>85</v>
+      <c r="C4" s="12">
+        <v>58644.27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="10">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
         <v>0.7</v>
       </c>
-      <c r="B5" s="6">
-        <f>B4+40</f>
-        <v>180</v>
+      <c r="B5" s="10">
+        <v>3531.65</v>
       </c>
-      <c r="C5" s="8">
-        <f>C4+10</f>
-        <v>95</v>
+      <c r="C5" s="11">
+        <v>93826.36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8">
         <v>0.9</v>
       </c>
-      <c r="B6" s="6">
-        <f>B5+40</f>
-        <v>220</v>
+      <c r="B6" s="13">
+        <v>3531.65</v>
       </c>
-      <c r="C6" s="8">
-        <f>C5+10</f>
-        <v>105</v>
+      <c r="C6" s="14">
+        <v>84233.8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
-        <v>100</v>
+      <c r="B11" s="10">
+        <v>3502.57</v>
       </c>
-      <c r="C11" s="5">
-        <v>105</v>
+      <c r="C11" s="10">
+        <v>65300.68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>4</v>
       </c>
-      <c r="B12" s="2">
-        <f>B11+30</f>
-        <v>130</v>
+      <c r="B12" s="1">
+        <v>3504.47</v>
       </c>
-      <c r="C12" s="6">
-        <f>C11+20</f>
-        <v>125</v>
+      <c r="C12" s="1">
+        <v>54212.800000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="10">
+        <v>3506.1</v>
+      </c>
+      <c r="C13" s="10">
+        <v>54328.05</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
-        <f>B12+30</f>
-        <v>160</v>
+      <c r="B14" s="15">
+        <v>3506.1</v>
       </c>
-      <c r="C14" s="6">
-        <f>C12+20</f>
-        <v>145</v>
+      <c r="C14" s="15">
+        <v>54949.62</v>
       </c>
     </row>
-    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" s="3">
+        <f>C3-C11</f>
+        <v>114408.41</v>
+      </c>
+      <c r="C16" s="3">
+        <f>AVERAGE(B16:B19)</f>
+        <v>46905.592499999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:B20" si="0">C4-C12</f>
+        <v>4431.4699999999939</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>39498.31</v>
+      </c>
+      <c r="C18" s="3">
+        <f>AVERAGE(Table1[Consumo de Datos '[kB']])</f>
+        <v>3531.6524999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>29284.18</v>
+      </c>
+      <c r="C19" s="3">
+        <f>AVERAGE(Table13[Consumo de Datos '[kB']])</f>
+        <v>3504.81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a4df9e4b793c0fa050084ef4feafa589">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="067b7080d2289f9ba15465beea7d18a8" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -3689,27 +5778,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF363B8-2236-4100-84F9-92CAF618B773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3726,29 +5820,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>